<commit_message>
updates in clips inventory
</commit_message>
<xml_diff>
--- a/Clips_Inventory_16.xlsx
+++ b/Clips_Inventory_16.xlsx
@@ -27941,10 +27941,10 @@
   <dimension ref="A1:BL470"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="5" ySplit="2" topLeftCell="AC3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="5" ySplit="2" topLeftCell="AG3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="AD139" sqref="AD139"/>
+      <selection pane="bottomRight" activeCell="AI4" sqref="AI4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -28246,7 +28246,7 @@
       </c>
       <c r="C4" s="8">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D4" s="7">
         <f t="shared" ref="D4:E67" si="1">SUM(BB4-F4-J4-N4-R4-V4-Z4-AD4-AH4-AL4-AP4-AT4-AX4)</f>
@@ -28254,7 +28254,10 @@
       </c>
       <c r="E4" s="12">
         <f t="shared" si="1"/>
-        <v>3</v>
+        <v>2</v>
+      </c>
+      <c r="AI4">
+        <v>1</v>
       </c>
       <c r="BB4" s="9">
         <f>'2015'!D4</f>
@@ -29272,7 +29275,7 @@
       </c>
       <c r="C34" s="8">
         <f t="shared" si="0"/>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D34" s="7">
         <f t="shared" si="1"/>
@@ -29280,7 +29283,7 @@
       </c>
       <c r="E34" s="7">
         <f t="shared" si="1"/>
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="G34" s="1">
         <v>1</v>
@@ -29295,6 +29298,9 @@
         <v>1</v>
       </c>
       <c r="AE34">
+        <v>1</v>
+      </c>
+      <c r="AI34">
         <v>1</v>
       </c>
       <c r="BB34" s="9">
@@ -29535,15 +29541,15 @@
       </c>
       <c r="C41" s="8">
         <f t="shared" si="0"/>
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="D41" s="7">
         <f t="shared" si="1"/>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E41" s="7">
         <f t="shared" si="1"/>
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F41" s="1">
         <v>1</v>
@@ -29561,6 +29567,9 @@
         <v>1</v>
       </c>
       <c r="AD41">
+        <v>2</v>
+      </c>
+      <c r="AI41">
         <v>1</v>
       </c>
       <c r="BB41" s="9">
@@ -29652,15 +29661,15 @@
       </c>
       <c r="C44" s="8">
         <f t="shared" si="0"/>
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="D44" s="7">
         <f t="shared" si="1"/>
-        <v>2</v>
-      </c>
-      <c r="E44" s="7">
+        <v>1</v>
+      </c>
+      <c r="E44" s="12">
         <f t="shared" si="1"/>
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="N44" s="1">
         <v>1</v>
@@ -29668,8 +29677,11 @@
       <c r="V44">
         <v>1</v>
       </c>
+      <c r="AD44">
+        <v>1</v>
+      </c>
       <c r="AE44">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="BB44" s="9">
         <f>'2015'!D44</f>
@@ -29690,7 +29702,7 @@
       </c>
       <c r="C45" s="8">
         <f t="shared" si="0"/>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D45" s="7">
         <f t="shared" si="1"/>
@@ -29698,7 +29710,7 @@
       </c>
       <c r="E45" s="7">
         <f t="shared" si="1"/>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F45" s="1">
         <v>1</v>
@@ -29713,6 +29725,9 @@
         <v>1</v>
       </c>
       <c r="AD45">
+        <v>1</v>
+      </c>
+      <c r="AI45">
         <v>1</v>
       </c>
       <c r="BB45" s="9">
@@ -29830,7 +29845,7 @@
       </c>
       <c r="C49" s="8">
         <f t="shared" si="0"/>
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D49" s="7">
         <f t="shared" si="1"/>
@@ -29838,7 +29853,7 @@
       </c>
       <c r="E49" s="7">
         <f t="shared" si="1"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J49" s="1">
         <v>1</v>
@@ -29859,6 +29874,9 @@
         <v>2</v>
       </c>
       <c r="AE49">
+        <v>1</v>
+      </c>
+      <c r="AI49">
         <v>1</v>
       </c>
       <c r="BB49" s="9">
@@ -29880,7 +29898,7 @@
       </c>
       <c r="C50" s="8">
         <f t="shared" si="0"/>
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D50" s="7">
         <f t="shared" si="1"/>
@@ -29888,7 +29906,7 @@
       </c>
       <c r="E50" s="7">
         <f t="shared" si="1"/>
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F50" s="1">
         <v>1</v>
@@ -29901,6 +29919,9 @@
       </c>
       <c r="W50">
         <v>2</v>
+      </c>
+      <c r="AI50">
+        <v>1</v>
       </c>
       <c r="BB50" s="9">
         <f>'2015'!D50</f>
@@ -31632,11 +31653,11 @@
       </c>
       <c r="C102" s="8">
         <f t="shared" si="3"/>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D102" s="17">
         <f t="shared" si="4"/>
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E102" s="7">
         <f t="shared" si="4"/>
@@ -31646,7 +31667,7 @@
         <v>1</v>
       </c>
       <c r="AD102">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="BB102" s="9">
         <f>'2015'!D102</f>
@@ -32418,11 +32439,11 @@
       </c>
       <c r="C126" s="8">
         <f t="shared" si="3"/>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D126" s="7">
         <f t="shared" si="4"/>
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E126" s="7">
         <f t="shared" si="4"/>
@@ -32437,6 +32458,9 @@
       <c r="Z126">
         <v>1</v>
       </c>
+      <c r="AD126">
+        <v>1</v>
+      </c>
       <c r="BB126" s="9">
         <f>'2015'!D126</f>
         <v>6</v>
@@ -32957,7 +32981,7 @@
       </c>
       <c r="C142" s="8">
         <f t="shared" si="6"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D142" s="7">
         <f t="shared" si="7"/>
@@ -32965,9 +32989,12 @@
       </c>
       <c r="E142" s="12">
         <f t="shared" si="7"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="W142">
+        <v>1</v>
+      </c>
+      <c r="AI142">
         <v>1</v>
       </c>
       <c r="BB142" s="9">
@@ -33219,7 +33246,7 @@
       </c>
       <c r="C150" s="8">
         <f t="shared" si="6"/>
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="D150" s="12">
         <f t="shared" si="7"/>
@@ -33227,7 +33254,7 @@
       </c>
       <c r="E150" s="7">
         <f t="shared" si="7"/>
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F150" s="1">
         <v>3</v>
@@ -33257,6 +33284,9 @@
         <v>2</v>
       </c>
       <c r="AE150">
+        <v>1</v>
+      </c>
+      <c r="AI150">
         <v>1</v>
       </c>
       <c r="BB150" s="9">
@@ -33278,11 +33308,11 @@
       </c>
       <c r="C151" s="8">
         <f t="shared" si="6"/>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D151" s="7">
         <f t="shared" si="7"/>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E151" s="7">
         <f t="shared" si="7"/>
@@ -33294,6 +33324,9 @@
       <c r="V151">
         <v>2</v>
       </c>
+      <c r="AD151">
+        <v>1</v>
+      </c>
       <c r="BB151" s="9">
         <f>'2015'!D151</f>
         <v>6</v>
@@ -33962,7 +33995,7 @@
       </c>
       <c r="C172" s="8">
         <f t="shared" si="6"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D172" s="17">
         <f t="shared" si="7"/>
@@ -33970,9 +34003,12 @@
       </c>
       <c r="E172" s="17">
         <f t="shared" si="7"/>
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="R172">
+        <v>1</v>
+      </c>
+      <c r="AI172">
         <v>1</v>
       </c>
       <c r="BB172" s="9">
@@ -34026,7 +34062,7 @@
       </c>
       <c r="C174" s="8">
         <f t="shared" si="6"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D174" s="7">
         <f t="shared" si="7"/>
@@ -34034,9 +34070,12 @@
       </c>
       <c r="E174" s="7">
         <f t="shared" si="7"/>
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="J174" s="1">
+        <v>1</v>
+      </c>
+      <c r="AI174">
         <v>1</v>
       </c>
       <c r="BB174" s="9">
@@ -34285,11 +34324,11 @@
       </c>
       <c r="C182" s="8">
         <f t="shared" si="6"/>
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="D182" s="7">
         <f t="shared" si="7"/>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E182" s="7">
         <f t="shared" si="7"/>
@@ -34317,7 +34356,7 @@
         <v>3</v>
       </c>
       <c r="AD182">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AE182">
         <v>1</v>
@@ -34891,7 +34930,7 @@
       </c>
       <c r="C200" s="8">
         <f t="shared" si="9"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D200" s="7">
         <f t="shared" si="10"/>
@@ -34899,7 +34938,10 @@
       </c>
       <c r="E200" s="7">
         <f t="shared" si="10"/>
-        <v>5</v>
+        <v>4</v>
+      </c>
+      <c r="AE200">
+        <v>1</v>
       </c>
       <c r="BB200" s="9">
         <f>'2015'!D200</f>
@@ -34965,15 +35007,15 @@
       <c r="B203" s="13"/>
       <c r="C203" s="14">
         <f>SUM(C3:C201)</f>
-        <v>388</v>
+        <v>408</v>
       </c>
       <c r="D203" s="15">
         <f>SUM(D3:D201)</f>
-        <v>795</v>
+        <v>789</v>
       </c>
       <c r="E203" s="15">
         <f>SUM(E3:E201)</f>
-        <v>1233</v>
+        <v>1219</v>
       </c>
       <c r="F203" s="15">
         <f>SUM(F3:F201)</f>
@@ -35037,11 +35079,11 @@
       <c r="AC203" s="13"/>
       <c r="AD203" s="13">
         <f>SUM(AD3:AD201)</f>
-        <v>18</v>
+        <v>24</v>
       </c>
       <c r="AE203" s="13">
         <f>SUM(AE3:AE201)</f>
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="AF203" s="13"/>
       <c r="AG203" s="13"/>
@@ -35051,7 +35093,7 @@
       </c>
       <c r="AI203" s="13">
         <f>SUM(AI3:AI201)</f>
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="AJ203" s="13"/>
       <c r="AK203" s="13"/>
@@ -35180,7 +35222,7 @@
       <c r="D205" s="15"/>
       <c r="E205" s="15">
         <f>SUM(D203+E203)</f>
-        <v>2028</v>
+        <v>2008</v>
       </c>
       <c r="F205" s="15" t="s">
         <v>4</v>
@@ -35241,7 +35283,7 @@
       </c>
       <c r="AE205" s="13">
         <f>SUM(AD203:AE203)</f>
-        <v>33</v>
+        <v>43</v>
       </c>
       <c r="AF205" s="13"/>
       <c r="AG205" s="13"/>
@@ -35250,7 +35292,7 @@
       </c>
       <c r="AI205" s="13">
         <f>SUM(AH203:AI203)</f>
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="AJ205" s="13"/>
       <c r="AK205" s="13"/>

</xml_diff>

<commit_message>
update to clips inventory
</commit_message>
<xml_diff>
--- a/Clips_Inventory_16.xlsx
+++ b/Clips_Inventory_16.xlsx
@@ -27941,10 +27941,10 @@
   <dimension ref="A1:BL470"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="5" ySplit="2" topLeftCell="AG3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="5" ySplit="2" topLeftCell="AJ3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="AI4" sqref="AI4"/>
+      <selection pane="bottomRight" activeCell="AM51" sqref="AM51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -29097,7 +29097,7 @@
       </c>
       <c r="C29" s="8">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D29" s="7">
         <f t="shared" si="1"/>
@@ -29105,7 +29105,10 @@
       </c>
       <c r="E29" s="7">
         <f t="shared" si="1"/>
-        <v>4</v>
+        <v>3</v>
+      </c>
+      <c r="AI29">
+        <v>1</v>
       </c>
       <c r="BB29" s="9">
         <f>'2015'!D29</f>
@@ -29354,7 +29357,7 @@
       </c>
       <c r="C36" s="8">
         <f t="shared" si="0"/>
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D36" s="7">
         <f t="shared" si="1"/>
@@ -29362,7 +29365,7 @@
       </c>
       <c r="E36" s="7">
         <f t="shared" si="1"/>
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="G36" s="1">
         <v>1</v>
@@ -29386,6 +29389,9 @@
         <v>1</v>
       </c>
       <c r="AD36">
+        <v>1</v>
+      </c>
+      <c r="AI36">
         <v>1</v>
       </c>
       <c r="BB36" s="9">
@@ -29541,7 +29547,7 @@
       </c>
       <c r="C41" s="8">
         <f t="shared" si="0"/>
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D41" s="7">
         <f t="shared" si="1"/>
@@ -29549,7 +29555,7 @@
       </c>
       <c r="E41" s="7">
         <f t="shared" si="1"/>
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F41" s="1">
         <v>1</v>
@@ -29570,7 +29576,7 @@
         <v>2</v>
       </c>
       <c r="AI41">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="BB41" s="9">
         <f>'2015'!D41</f>
@@ -29702,7 +29708,7 @@
       </c>
       <c r="C45" s="8">
         <f t="shared" si="0"/>
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D45" s="7">
         <f t="shared" si="1"/>
@@ -29710,7 +29716,7 @@
       </c>
       <c r="E45" s="7">
         <f t="shared" si="1"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F45" s="1">
         <v>1</v>
@@ -29728,6 +29734,9 @@
         <v>1</v>
       </c>
       <c r="AI45">
+        <v>1</v>
+      </c>
+      <c r="AM45">
         <v>1</v>
       </c>
       <c r="BB45" s="9">
@@ -29942,7 +29951,7 @@
       </c>
       <c r="C51" s="8">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D51" s="17">
         <f t="shared" si="1"/>
@@ -29950,12 +29959,15 @@
       </c>
       <c r="E51" s="7">
         <f t="shared" si="1"/>
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="N51" s="1">
         <v>1</v>
       </c>
       <c r="R51">
+        <v>1</v>
+      </c>
+      <c r="AM51">
         <v>1</v>
       </c>
       <c r="BB51" s="9">
@@ -30466,7 +30478,7 @@
       </c>
       <c r="C65" s="8">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D65" s="7">
         <f t="shared" si="1"/>
@@ -30474,12 +30486,15 @@
       </c>
       <c r="E65" s="7">
         <f t="shared" si="1"/>
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F65" s="1">
         <v>1</v>
       </c>
       <c r="V65">
+        <v>1</v>
+      </c>
+      <c r="AI65">
         <v>1</v>
       </c>
       <c r="BB65" s="9">
@@ -31464,7 +31479,7 @@
       </c>
       <c r="C96" s="8">
         <f t="shared" si="3"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D96" s="7">
         <f t="shared" si="4"/>
@@ -31472,9 +31487,12 @@
       </c>
       <c r="E96" s="7">
         <f t="shared" si="4"/>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="K96" s="1">
+        <v>1</v>
+      </c>
+      <c r="AI96">
         <v>1</v>
       </c>
       <c r="BB96" s="9">
@@ -32203,7 +32221,7 @@
       </c>
       <c r="C119" s="8">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D119" s="7">
         <f t="shared" si="4"/>
@@ -32211,7 +32229,10 @@
       </c>
       <c r="E119" s="7">
         <f t="shared" si="4"/>
-        <v>4</v>
+        <v>3</v>
+      </c>
+      <c r="AM119">
+        <v>1</v>
       </c>
       <c r="BB119" s="9">
         <f>'2015'!D119</f>
@@ -32360,7 +32381,7 @@
       </c>
       <c r="C124" s="8">
         <f t="shared" si="3"/>
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D124" s="7">
         <f t="shared" si="4"/>
@@ -32368,7 +32389,7 @@
       </c>
       <c r="E124" s="7">
         <f t="shared" si="4"/>
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F124" s="1">
         <v>1</v>
@@ -32390,6 +32411,9 @@
       </c>
       <c r="W124">
         <v>2</v>
+      </c>
+      <c r="AI124">
+        <v>1</v>
       </c>
       <c r="BB124" s="9">
         <f>'2015'!D124</f>
@@ -32439,7 +32463,7 @@
       </c>
       <c r="C126" s="8">
         <f t="shared" si="3"/>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D126" s="7">
         <f t="shared" si="4"/>
@@ -32447,7 +32471,7 @@
       </c>
       <c r="E126" s="7">
         <f t="shared" si="4"/>
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="K126" s="1">
         <v>1</v>
@@ -32459,6 +32483,9 @@
         <v>1</v>
       </c>
       <c r="AD126">
+        <v>1</v>
+      </c>
+      <c r="AM126">
         <v>1</v>
       </c>
       <c r="BB126" s="9">
@@ -33346,7 +33373,7 @@
       </c>
       <c r="C152" s="8">
         <f t="shared" si="6"/>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D152" s="17">
         <f t="shared" si="7"/>
@@ -33354,7 +33381,7 @@
       </c>
       <c r="E152" s="7">
         <f t="shared" si="7"/>
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G152" s="1">
         <v>1</v>
@@ -33366,6 +33393,9 @@
         <v>2</v>
       </c>
       <c r="Z152">
+        <v>1</v>
+      </c>
+      <c r="AM152">
         <v>1</v>
       </c>
       <c r="BB152" s="9">
@@ -33387,7 +33417,7 @@
       </c>
       <c r="C153" s="8">
         <f t="shared" si="6"/>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D153" s="7">
         <f t="shared" si="7"/>
@@ -33395,7 +33425,7 @@
       </c>
       <c r="E153" s="7">
         <f t="shared" si="7"/>
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="N153" s="1">
         <v>1</v>
@@ -33404,6 +33434,9 @@
         <v>1</v>
       </c>
       <c r="Z153">
+        <v>1</v>
+      </c>
+      <c r="AM153">
         <v>1</v>
       </c>
       <c r="BB153" s="9">
@@ -35007,7 +35040,7 @@
       <c r="B203" s="13"/>
       <c r="C203" s="14">
         <f>SUM(C3:C201)</f>
-        <v>408</v>
+        <v>420</v>
       </c>
       <c r="D203" s="15">
         <f>SUM(D3:D201)</f>
@@ -35015,7 +35048,7 @@
       </c>
       <c r="E203" s="15">
         <f>SUM(E3:E201)</f>
-        <v>1219</v>
+        <v>1207</v>
       </c>
       <c r="F203" s="15">
         <f>SUM(F3:F201)</f>
@@ -35093,7 +35126,7 @@
       </c>
       <c r="AI203" s="13">
         <f>SUM(AI3:AI201)</f>
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="AJ203" s="13"/>
       <c r="AK203" s="13"/>
@@ -35103,7 +35136,7 @@
       </c>
       <c r="AM203" s="13">
         <f>SUM(AM3:AM201)</f>
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="AN203" s="13"/>
       <c r="AO203" s="13"/>
@@ -35222,7 +35255,7 @@
       <c r="D205" s="15"/>
       <c r="E205" s="15">
         <f>SUM(D203+E203)</f>
-        <v>2008</v>
+        <v>1996</v>
       </c>
       <c r="F205" s="15" t="s">
         <v>4</v>
@@ -35292,7 +35325,7 @@
       </c>
       <c r="AI205" s="13">
         <f>SUM(AH203:AI203)</f>
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="AJ205" s="13"/>
       <c r="AK205" s="13"/>
@@ -35301,7 +35334,7 @@
       </c>
       <c r="AM205" s="13">
         <f>SUM(AL203:AM203)</f>
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="AN205" s="13"/>
       <c r="AO205" s="13"/>

</xml_diff>